<commit_message>
testing of file upload complete
</commit_message>
<xml_diff>
--- a/data/uploaded_excel_files/uploaded_file.xlsx
+++ b/data/uploaded_excel_files/uploaded_file.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_71424A7A5C5706DB7F74F84FD1238614B5F1CF49" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{72E707BE-0160-4B47-9423-3E839962E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83EA49F-FD48-4F55-B28D-B1775F13EF54}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1740" windowWidth="24870" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="3390" windowWidth="18825" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
-    <sheet name="VM-Data" sheetId="2" r:id="rId2"/>
-    <sheet name="MegaPort" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="WS-Data" sheetId="1" r:id="rId2"/>
+    <sheet name="VM-Data" sheetId="2" r:id="rId3"/>
+    <sheet name="MegaPort" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>Customer: 1038</t>
   </si>
@@ -46,7 +47,7 @@
     <t>Total Secs:</t>
   </si>
   <si>
-    <t>Analysis Window: Mon,Tue,Wed,Th,Fri, 20:00 to 8:00</t>
+    <t>Analysis Window: Mon,Tue,Wed,Th,Fri, 8:00 to 20:00</t>
   </si>
   <si>
     <t>Host Name</t>
@@ -360,6 +361,9 @@
     <t>ld71r16u14ws</t>
   </si>
   <si>
+    <t>4m</t>
+  </si>
+  <si>
     <t>ld71r18u44ews</t>
   </si>
   <si>
@@ -406,13 +410,22 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>6m</t>
+  </si>
+  <si>
+    <t>8m</t>
+  </si>
+  <si>
+    <t>2m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,6 +436,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -764,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -819,6 +838,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -836,8 +856,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -848,6 +866,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -871,6 +891,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1169,17 +1193,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1087BDBF-61A9-4E89-AA68-4C3AF5657CC8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AG11" sqref="A11:AG11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
@@ -1207,7 +1242,7 @@
     <col min="38" max="43" width="12.28515625" style="1" customWidth="1"/>
     <col min="44" max="44" width="7.5703125" style="1" customWidth="1"/>
     <col min="45" max="45" width="4.42578125" style="1" customWidth="1"/>
-    <col min="46" max="46" width="5.7109375" style="1" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" style="1" customWidth="1"/>
     <col min="47" max="47" width="9" style="1" customWidth="1"/>
     <col min="48" max="48" width="5.85546875" style="1" customWidth="1"/>
     <col min="49" max="49" width="5.7109375" style="1" customWidth="1"/>
@@ -1235,16 +1270,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1257,96 +1292,96 @@
         <v>3</v>
       </c>
       <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="38" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="26" t="s">
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="30" t="s">
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="22"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="22"/>
-      <c r="AQ4" s="23"/>
-      <c r="AR4" s="28" t="s">
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="25"/>
-      <c r="AY4" s="29"/>
-      <c r="AZ4" s="24" t="s">
+      <c r="AS4" s="26"/>
+      <c r="AT4" s="26"/>
+      <c r="AU4" s="26"/>
+      <c r="AV4" s="26"/>
+      <c r="AW4" s="26"/>
+      <c r="AX4" s="26"/>
+      <c r="AY4" s="30"/>
+      <c r="AZ4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="BA4" s="25"/>
-      <c r="BB4" s="25"/>
-      <c r="BC4" s="25"/>
-      <c r="BD4" s="25"/>
-      <c r="BE4" s="25"/>
-      <c r="BF4" s="25"/>
-      <c r="BG4" s="25"/>
-      <c r="BH4" s="25"/>
-      <c r="BI4" s="25"/>
-      <c r="BJ4" s="25"/>
-      <c r="BK4" s="25"/>
-      <c r="BL4" s="25"/>
-      <c r="BM4" s="25"/>
-      <c r="BN4" s="25"/>
+      <c r="BA4" s="26"/>
+      <c r="BB4" s="26"/>
+      <c r="BC4" s="26"/>
+      <c r="BD4" s="26"/>
+      <c r="BE4" s="26"/>
+      <c r="BF4" s="26"/>
+      <c r="BG4" s="26"/>
+      <c r="BH4" s="26"/>
+      <c r="BI4" s="26"/>
+      <c r="BJ4" s="26"/>
+      <c r="BK4" s="26"/>
+      <c r="BL4" s="26"/>
+      <c r="BM4" s="26"/>
+      <c r="BN4" s="26"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -1549,13 +1584,13 @@
         <v>24</v>
       </c>
       <c r="D6" s="18">
-        <v>0.15625000000001421</v>
+        <v>3.17361111111112</v>
       </c>
       <c r="E6" s="18">
-        <v>68.836805555555557</v>
+        <v>67.708333333333343</v>
       </c>
       <c r="F6" s="18">
-        <v>0.74882419582904447</v>
+        <v>39.815863962563</v>
       </c>
       <c r="G6" s="18">
         <v>0</v>
@@ -1565,13 +1600,13 @@
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18">
-        <v>9.5491416193738132E-4</v>
+        <v>2.0131762049196702</v>
       </c>
       <c r="K6" s="18">
-        <v>34.862557870370381</v>
+        <v>28.9639756944444</v>
       </c>
       <c r="L6" s="18">
-        <v>0.1068956176778499</v>
+        <v>18.0807847747114</v>
       </c>
       <c r="M6" s="18">
         <v>0</v>
@@ -1587,34 +1622,34 @@
         <v>68.410642432000003</v>
       </c>
       <c r="R6" s="18">
-        <v>6.2241132207352052</v>
+        <v>11.55436561183733</v>
       </c>
       <c r="S6" s="18">
-        <v>16.33349233798933</v>
+        <v>16.446132777050551</v>
       </c>
       <c r="T6" s="18">
-        <v>11.83482979649345</v>
+        <v>12.51275537020771</v>
       </c>
       <c r="U6" s="18">
         <v>0</v>
       </c>
       <c r="V6" s="18">
-        <v>6.1908888888888888E-4</v>
+        <v>6.5433333333333326E-4</v>
       </c>
       <c r="W6" s="18">
-        <v>0.3959353888888888</v>
+        <v>1.289013722222222</v>
       </c>
       <c r="X6" s="18">
-        <v>1.0173492720154209E-3</v>
+        <v>2.1589043077038521E-3</v>
       </c>
       <c r="Y6" s="18">
-        <v>4.4499999999999991E-5</v>
+        <v>4.5466666666666663E-5</v>
       </c>
       <c r="Z6" s="18">
-        <v>0.79352971111111104</v>
+        <v>7.6640584888888874</v>
       </c>
       <c r="AA6" s="18">
-        <v>1.3771284216603421E-3</v>
+        <v>6.9775276762525018E-3</v>
       </c>
       <c r="AB6" s="18">
         <v>832.18466837788742</v>
@@ -1663,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="AT6" s="18">
-        <v>0</v>
+        <v>20.1234</v>
       </c>
       <c r="AU6" s="18">
         <v>0</v>
@@ -1672,10 +1707,10 @@
         <v>1</v>
       </c>
       <c r="AW6" s="18">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AX6" s="18">
-        <v>28.89076923076918</v>
+        <v>29.442564102564109</v>
       </c>
       <c r="AY6" s="18">
         <v>0</v>
@@ -1684,46 +1719,46 @@
         <v>0</v>
       </c>
       <c r="BA6" s="18">
-        <v>29.70620017777777</v>
+        <v>22.264166400000001</v>
       </c>
       <c r="BB6" s="18">
-        <v>1.955131286292288E-2</v>
+        <v>2.6786931844974399E-2</v>
       </c>
       <c r="BC6" s="18">
-        <v>3.6067555555555548E-3</v>
+        <v>4.7274666666666659E-3</v>
       </c>
       <c r="BD6" s="18">
         <v>109.4738545777778</v>
       </c>
       <c r="BE6" s="18">
-        <v>0.21013705905293259</v>
+        <v>0.19570285034240509</v>
       </c>
       <c r="BF6" s="18">
         <v>0</v>
       </c>
       <c r="BG6" s="18">
-        <v>1132.8111111111109</v>
+        <v>387.61111111111109</v>
       </c>
       <c r="BH6" s="18">
-        <v>0.75199433336034827</v>
+        <v>0.69459248778285854</v>
       </c>
       <c r="BI6" s="18">
-        <v>0.22222222222222221</v>
+        <v>0.25555555555555548</v>
       </c>
       <c r="BJ6" s="18">
         <v>3433.177777777777</v>
       </c>
       <c r="BK6" s="18">
-        <v>8.2236388399206373</v>
+        <v>7.6584782609093116</v>
       </c>
       <c r="BL6" s="18">
-        <v>1934364.770304</v>
+        <v>1934804.1236479999</v>
       </c>
       <c r="BM6" s="18">
-        <v>1938809.6839680001</v>
+        <v>1938792.9067520001</v>
       </c>
       <c r="BN6" s="18">
-        <v>1938213.791401617</v>
+        <v>1937925.9434430359</v>
       </c>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
@@ -1735,72 +1770,76 @@
         <v>28</v>
       </c>
       <c r="D7" s="20">
-        <v>6.9444444444457076E-2</v>
+        <v>1.55555555555557</v>
       </c>
       <c r="E7" s="20">
-        <v>40.295134548611109</v>
+        <v>88.2638888888889</v>
       </c>
       <c r="F7" s="20">
-        <v>0.69630361859861978</v>
+        <v>24.7140567507901</v>
       </c>
       <c r="G7" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="20">
-        <v>0</v>
-      </c>
-      <c r="I7" s="20"/>
+        <v>120</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="J7" s="20">
-        <v>1.860119047620401E-2</v>
+        <v>9.0626240079365008</v>
       </c>
       <c r="K7" s="20">
-        <v>22.603564034598211</v>
+        <v>89.690228174603106</v>
       </c>
       <c r="L7" s="20">
-        <v>0.16420847012619791</v>
+        <v>89.132013670350801</v>
       </c>
       <c r="M7" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="20">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="O7" s="20">
-        <v>0</v>
-      </c>
-      <c r="P7" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="Q7" s="20">
         <v>137.15297484800001</v>
       </c>
       <c r="R7" s="20">
-        <v>2.9437461319920288</v>
+        <v>6.9375566622197482</v>
       </c>
       <c r="S7" s="20">
-        <v>9.6522871564918518</v>
+        <v>9.765903521118787</v>
       </c>
       <c r="T7" s="20">
-        <v>7.0211528958709692</v>
+        <v>7.3678552547746534</v>
       </c>
       <c r="U7" s="20">
         <v>0</v>
       </c>
       <c r="V7" s="20">
-        <v>6.6505555555555545E-4</v>
+        <v>7.3543333333333323E-4</v>
       </c>
       <c r="W7" s="20">
-        <v>1.348351111111111E-2</v>
+        <v>1.8675351</v>
       </c>
       <c r="X7" s="20">
-        <v>8.8058666066642179E-4</v>
+        <v>2.226264855098132E-3</v>
       </c>
       <c r="Y7" s="20">
-        <v>1.093444444444444E-4</v>
+        <v>1.107666666666667E-4</v>
       </c>
       <c r="Z7" s="20">
-        <v>0.81337996666666657</v>
+        <v>1.186898133333333</v>
       </c>
       <c r="AA7" s="20">
-        <v>2.0486787357623069E-3</v>
+        <v>2.1609552893814771E-3</v>
       </c>
       <c r="AB7" s="20">
         <v>632.02655480675276</v>
@@ -1849,7 +1888,7 @@
         <v>3</v>
       </c>
       <c r="AT7" s="20">
-        <v>5.6410256410256406E-3</v>
+        <v>13.54321</v>
       </c>
       <c r="AU7" s="20">
         <v>0</v>
@@ -1858,10 +1897,10 @@
         <v>1</v>
       </c>
       <c r="AW7" s="20">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AX7" s="20">
-        <v>28.429743589743609</v>
+        <v>28.443076923076951</v>
       </c>
       <c r="AY7" s="20">
         <v>0</v>
@@ -1870,46 +1909,46 @@
         <v>0</v>
       </c>
       <c r="BA7" s="20">
-        <v>15.55046857735111</v>
+        <v>11.65377991111111</v>
       </c>
       <c r="BB7" s="20">
-        <v>2.0969029559861008E-2</v>
+        <v>2.7487692632569539E-2</v>
       </c>
       <c r="BC7" s="20">
-        <v>3.5498666666666659E-3</v>
+        <v>4.8696888888888883E-3</v>
       </c>
       <c r="BD7" s="20">
-        <v>7.7861774222222211</v>
+        <v>33.580464355555549</v>
       </c>
       <c r="BE7" s="20">
-        <v>4.6014516634384939E-2</v>
+        <v>0.10158826014927549</v>
       </c>
       <c r="BF7" s="20">
         <v>0</v>
       </c>
       <c r="BG7" s="20">
-        <v>339.69917583333341</v>
+        <v>361.13333333333333</v>
       </c>
       <c r="BH7" s="20">
-        <v>0.47951025211949422</v>
+        <v>0.79715668604607093</v>
       </c>
       <c r="BI7" s="20">
-        <v>0.3</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BJ7" s="20">
-        <v>366.21111111111111</v>
+        <v>2235.1111111111109</v>
       </c>
       <c r="BK7" s="20">
-        <v>3.1639327313050249</v>
+        <v>5.7751855397173024</v>
       </c>
       <c r="BL7" s="20">
-        <v>884350.12403199996</v>
+        <v>884693.00838400004</v>
       </c>
       <c r="BM7" s="20">
-        <v>888922.96396800003</v>
+        <v>888918.76966400002</v>
       </c>
       <c r="BN7" s="20">
-        <v>888417.29235941754</v>
+        <v>888200.19115139288</v>
       </c>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.25">
@@ -1921,13 +1960,13 @@
         <v>24</v>
       </c>
       <c r="D8" s="18">
-        <v>0.34722222222222848</v>
+        <v>2.3298611111111098</v>
       </c>
       <c r="E8" s="18">
-        <v>59.079861111111107</v>
+        <v>76.475694444444443</v>
       </c>
       <c r="F8" s="18">
-        <v>8.9902504583559875</v>
+        <v>13.922552346485629</v>
       </c>
       <c r="G8" s="18">
         <v>0</v>
@@ -1937,13 +1976,13 @@
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="18">
-        <v>2.0254629629647521E-2</v>
+        <v>3.7615740740747597E-2</v>
       </c>
       <c r="K8" s="18">
-        <v>16.71947337962963</v>
+        <v>25.69073266601562</v>
       </c>
       <c r="L8" s="18">
-        <v>1.4089254113336549</v>
+        <v>15.3746751110908</v>
       </c>
       <c r="M8" s="18">
         <v>0</v>
@@ -1959,34 +1998,34 @@
         <v>68.410642432000003</v>
       </c>
       <c r="R8" s="18">
-        <v>19.63934822181324</v>
+        <v>11.45298742047048</v>
       </c>
       <c r="S8" s="18">
-        <v>28.359417421469772</v>
+        <v>33.192759805714559</v>
       </c>
       <c r="T8" s="18">
-        <v>21.611791309123941</v>
+        <v>22.170397502779021</v>
       </c>
       <c r="U8" s="18">
         <v>0</v>
       </c>
       <c r="V8" s="18">
-        <v>6.8969999999999991E-4</v>
+        <v>7.1696666666666662E-4</v>
       </c>
       <c r="W8" s="18">
-        <v>0.68740926666666657</v>
+        <v>7.0244920888888887</v>
       </c>
       <c r="X8" s="18">
-        <v>4.2557420478100466E-3</v>
+        <v>1.418143975873829E-2</v>
       </c>
       <c r="Y8" s="18">
-        <v>5.5722222222222218E-5</v>
+        <v>6.3855555555555543E-5</v>
       </c>
       <c r="Z8" s="18">
-        <v>3.1942161885928861</v>
+        <v>5.6981399555555541</v>
       </c>
       <c r="AA8" s="18">
-        <v>7.3796257527600989E-3</v>
+        <v>1.1291403343945929E-2</v>
       </c>
       <c r="AB8" s="18">
         <v>3757.863341558264</v>
@@ -1998,34 +2037,34 @@
         <v>0</v>
       </c>
       <c r="AE8" s="18">
-        <v>2.5119168990637451E-2</v>
+        <v>9.8943070777222211E-2</v>
       </c>
       <c r="AF8" s="18">
-        <v>3.0900041237648833E-5</v>
+        <v>2.031529892100265E-3</v>
       </c>
       <c r="AG8" s="18">
-        <v>478.69856119947968</v>
+        <v>478.69874958113883</v>
       </c>
       <c r="AH8" s="18">
         <v>0</v>
       </c>
       <c r="AI8" s="18">
-        <v>3.479258694058042E-4</v>
+        <v>8.7083333333333318E-3</v>
       </c>
       <c r="AJ8" s="18">
-        <v>5.2801384613403058E-7</v>
+        <v>4.5228257884255552E-4</v>
       </c>
       <c r="AK8" s="18">
-        <v>106.40833726871681</v>
+        <v>106.4083749559543</v>
       </c>
       <c r="AL8" s="18">
         <v>0</v>
       </c>
       <c r="AM8" s="18">
-        <v>8.235294117647058</v>
+        <v>52.979066022544288</v>
       </c>
       <c r="AN8" s="18">
-        <v>2.537826422720852</v>
+        <v>0.77324127458075387</v>
       </c>
       <c r="AO8" s="18">
         <v>0</v>
@@ -2034,16 +2073,16 @@
         <v>9.8799313893653515</v>
       </c>
       <c r="AQ8" s="18">
-        <v>3.454410747613883</v>
+        <v>8.85484379787249E-2</v>
       </c>
       <c r="AR8" s="18">
         <v>0</v>
       </c>
       <c r="AS8" s="18">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="AT8" s="18">
-        <v>1.901025641025657</v>
+        <v>4.1210877373013304</v>
       </c>
       <c r="AU8" s="18">
         <v>0</v>
@@ -2052,10 +2091,10 @@
         <v>0</v>
       </c>
       <c r="AW8" s="18">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AX8" s="18">
-        <v>15.935384615384651</v>
+        <v>13.45253976398152</v>
       </c>
       <c r="AY8" s="18">
         <v>0</v>
@@ -2064,46 +2103,46 @@
         <v>0</v>
       </c>
       <c r="BA8" s="18">
-        <v>18.104553244444439</v>
+        <v>37.109942044444438</v>
       </c>
       <c r="BB8" s="18">
-        <v>3.2748740026090302E-2</v>
+        <v>5.5135872041485928E-2</v>
       </c>
       <c r="BC8" s="18">
-        <v>1.456924444444444E-2</v>
+        <v>1.2674844444444441E-2</v>
       </c>
       <c r="BD8" s="18">
-        <v>36.786949688888882</v>
+        <v>29.74225066666666</v>
       </c>
       <c r="BE8" s="18">
-        <v>0.1085857460549525</v>
+        <v>0.13620209581200021</v>
       </c>
       <c r="BF8" s="18">
         <v>0</v>
       </c>
       <c r="BG8" s="18">
-        <v>255.21111111111111</v>
+        <v>1174.633333333333</v>
       </c>
       <c r="BH8" s="18">
-        <v>0.87855038710517819</v>
+        <v>1.514983025775233</v>
       </c>
       <c r="BI8" s="18">
         <v>0.7</v>
       </c>
       <c r="BJ8" s="18">
-        <v>1151.955555555556</v>
+        <v>773.93333333333328</v>
       </c>
       <c r="BK8" s="18">
-        <v>6.9015480283094366</v>
+        <v>9.9537944315351616</v>
       </c>
       <c r="BL8" s="18">
-        <v>1901770.8339199999</v>
+        <v>1901783.416832</v>
       </c>
       <c r="BM8" s="18">
-        <v>1908769.030144</v>
+        <v>1908370.5712639999</v>
       </c>
       <c r="BN8" s="18">
-        <v>1903985.1663044919</v>
+        <v>1903922.5645696661</v>
       </c>
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.25">
@@ -2118,10 +2157,10 @@
         <v>0.2604166666666714</v>
       </c>
       <c r="E9" s="20">
-        <v>79.479166666666671</v>
+        <v>63.871527777777779</v>
       </c>
       <c r="F9" s="20">
-        <v>0.62445190121233907</v>
+        <v>0.460464852049355</v>
       </c>
       <c r="G9" s="20">
         <v>0</v>
@@ -2131,56 +2170,58 @@
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20">
-        <v>3.782242063493868E-2</v>
+        <v>2.03658234126986</v>
       </c>
       <c r="K9" s="20">
-        <v>70.640500992063494</v>
+        <v>97.5086805555555</v>
       </c>
       <c r="L9" s="20">
-        <v>0.27448259692167198</v>
+        <v>79.128619426852694</v>
       </c>
       <c r="M9" s="20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N9" s="20">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="O9" s="20">
-        <v>0</v>
-      </c>
-      <c r="P9" s="20"/>
+        <v>5</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>101</v>
+      </c>
       <c r="Q9" s="20">
         <v>137.15297484800001</v>
       </c>
       <c r="R9" s="20">
-        <v>3.7216138648518888</v>
+        <v>5.7300587586304204</v>
       </c>
       <c r="S9" s="20">
-        <v>8.983344081055975</v>
+        <v>9.1072159024206201</v>
       </c>
       <c r="T9" s="20">
-        <v>6.5792488981737023</v>
+        <v>6.815193461837012</v>
       </c>
       <c r="U9" s="20">
         <v>0</v>
       </c>
       <c r="V9" s="20">
-        <v>2.8679999999999998E-4</v>
+        <v>6.8722222222222221E-4</v>
       </c>
       <c r="W9" s="20">
-        <v>9.8065058380555556E-2</v>
+        <v>1.8828557666666661</v>
       </c>
       <c r="X9" s="20">
-        <v>1.0410184206415449E-3</v>
+        <v>2.0621695673197242E-3</v>
       </c>
       <c r="Y9" s="20">
-        <v>1.072111111111111E-4</v>
+        <v>1.093444444444444E-4</v>
       </c>
       <c r="Z9" s="20">
-        <v>1.2454098111111109</v>
+        <v>7.9400791111111104</v>
       </c>
       <c r="AA9" s="20">
-        <v>4.6053594567783372E-3</v>
+        <v>6.2541712494126427E-3</v>
       </c>
       <c r="AB9" s="20">
         <v>859.6917818945999</v>
@@ -2192,25 +2233,25 @@
         <v>0</v>
       </c>
       <c r="AE9" s="20">
-        <v>6.4541573825000004E-2</v>
+        <v>8.6998269000000003E-2</v>
       </c>
       <c r="AF9" s="20">
-        <v>8.8321268545122863E-5</v>
+        <v>4.4614496923076923E-5</v>
       </c>
       <c r="AG9" s="20">
-        <v>32.565560217058028</v>
+        <v>32.565571826143312</v>
       </c>
       <c r="AH9" s="20">
         <v>0</v>
       </c>
       <c r="AI9" s="20">
-        <v>3.2829285888888891E-3</v>
+        <v>3.714896972222223E-3</v>
       </c>
       <c r="AJ9" s="20">
-        <v>5.1105866298956716E-6</v>
+        <v>1.90507537037037E-6</v>
       </c>
       <c r="AK9" s="20">
-        <v>1.7074521391126749</v>
+        <v>1.707452728028479</v>
       </c>
       <c r="AL9" s="20">
         <v>0</v>
@@ -2225,19 +2266,19 @@
         <v>0</v>
       </c>
       <c r="AP9" s="20">
-        <v>0.3076292042657916</v>
+        <v>0</v>
       </c>
       <c r="AQ9" s="20">
-        <v>0.1025430680885972</v>
+        <v>0</v>
       </c>
       <c r="AR9" s="20">
         <v>0</v>
       </c>
       <c r="AS9" s="20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AT9" s="20">
-        <v>6.6769388803287113E-3</v>
+        <v>71.004615384615306</v>
       </c>
       <c r="AU9" s="20">
         <v>0</v>
@@ -2249,55 +2290,55 @@
         <v>83</v>
       </c>
       <c r="AX9" s="20">
-        <v>30.299435028248539</v>
+        <v>31.606666666666591</v>
       </c>
       <c r="AY9" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AZ9" s="20">
         <v>0</v>
       </c>
       <c r="BA9" s="20">
-        <v>57.886590816000002</v>
+        <v>17.026110577777779</v>
       </c>
       <c r="BB9" s="20">
-        <v>0.1184965992970063</v>
+        <v>2.9320953067251389E-2</v>
       </c>
       <c r="BC9" s="20">
-        <v>4.4145777777777773E-3</v>
+        <v>1.6839111111111109E-3</v>
       </c>
       <c r="BD9" s="20">
-        <v>40.494481830399998</v>
+        <v>23.070646044444441</v>
       </c>
       <c r="BE9" s="20">
-        <v>0.1897267189212013</v>
+        <v>0.17969634464722081</v>
       </c>
       <c r="BF9" s="20">
         <v>0</v>
       </c>
       <c r="BG9" s="20">
-        <v>1266.3703687499999</v>
+        <v>273.83333333333331</v>
       </c>
       <c r="BH9" s="20">
-        <v>2.4171464386852981</v>
+        <v>0.75590881945397248</v>
       </c>
       <c r="BI9" s="20">
-        <v>0.28888888888888892</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="BJ9" s="20">
-        <v>655.69999999999993</v>
+        <v>1027.211111111111</v>
       </c>
       <c r="BK9" s="20">
-        <v>6.0868747253725051</v>
+        <v>7.6325177993850479</v>
       </c>
       <c r="BL9" s="20">
-        <v>870601.19551999995</v>
+        <v>870311.78854400001</v>
       </c>
       <c r="BM9" s="20">
-        <v>883378.09407999995</v>
+        <v>883149.50451200001</v>
       </c>
       <c r="BN9" s="20">
-        <v>874612.64009898668</v>
+        <v>874526.4324986093</v>
       </c>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.25">
@@ -2309,72 +2350,76 @@
         <v>24</v>
       </c>
       <c r="D10" s="18">
-        <v>0.15625000000001421</v>
+        <v>16.1215277777777</v>
       </c>
       <c r="E10" s="18">
-        <v>35.208333333333343</v>
+        <v>98.2083333333333</v>
       </c>
       <c r="F10" s="18">
-        <v>1.4641387067728</v>
+        <v>72.7926838412546</v>
       </c>
       <c r="G10" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10" s="18">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18"/>
+        <v>360</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="J10" s="18">
-        <v>1.6637731481495169E-2</v>
+        <v>13.0224247685185</v>
       </c>
       <c r="K10" s="18">
-        <v>10.124421296296299</v>
+        <v>99.7157118055556</v>
       </c>
       <c r="L10" s="18">
-        <v>0.26564044207110271</v>
+        <v>76.9876</v>
       </c>
       <c r="M10" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N10" s="18">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="O10" s="18">
-        <v>0</v>
-      </c>
-      <c r="P10" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>101</v>
+      </c>
       <c r="Q10" s="18">
         <v>68.410642432000003</v>
       </c>
       <c r="R10" s="18">
-        <v>16.52170539289229</v>
+        <v>12.646701852858291</v>
       </c>
       <c r="S10" s="18">
-        <v>29.233088830993669</v>
+        <v>47.220886206572608</v>
       </c>
       <c r="T10" s="18">
-        <v>18.23871667406782</v>
+        <v>19.01565039801557</v>
       </c>
       <c r="U10" s="18">
         <v>0</v>
       </c>
       <c r="V10" s="18">
-        <v>6.9224444444444442E-4</v>
+        <v>6.9041111111111102E-4</v>
       </c>
       <c r="W10" s="18">
-        <v>6.0888244444444441E-2</v>
+        <v>0.28837618888888888</v>
       </c>
       <c r="X10" s="18">
-        <v>1.1001877272540409E-3</v>
+        <v>2.5309056242198489E-3</v>
       </c>
       <c r="Y10" s="18">
         <v>4.7399999999999987E-5</v>
       </c>
       <c r="Z10" s="18">
-        <v>2.4184207222222218</v>
+        <v>43.538736211111107</v>
       </c>
       <c r="AA10" s="18">
-        <v>3.8781591848160248E-3</v>
+        <v>5.8673473056466037E-2</v>
       </c>
       <c r="AB10" s="18">
         <v>803.94467463317835</v>
@@ -2386,55 +2431,55 @@
         <v>0</v>
       </c>
       <c r="AE10" s="18">
-        <v>5.6761999999999993E-2</v>
+        <v>0.1087134666666667</v>
       </c>
       <c r="AF10" s="18">
-        <v>1.8503299145299139E-4</v>
+        <v>1.051115616048647E-3</v>
       </c>
       <c r="AG10" s="18">
-        <v>243.63904273332199</v>
+        <v>243.64051476700189</v>
       </c>
       <c r="AH10" s="18">
         <v>0</v>
       </c>
       <c r="AI10" s="18">
-        <v>5.2072666666666666E-3</v>
+        <v>6.6842222222222216E-3</v>
       </c>
       <c r="AJ10" s="18">
-        <v>2.260125356125356E-5</v>
+        <v>1.3889645445318519E-4</v>
       </c>
       <c r="AK10" s="18">
-        <v>32.394014912822513</v>
+        <v>32.394211757693682</v>
       </c>
       <c r="AL10" s="18">
         <v>0</v>
       </c>
       <c r="AM10" s="18">
-        <v>1.5380908191359011E-2</v>
+        <v>0.52356020942408377</v>
       </c>
       <c r="AN10" s="18">
-        <v>1.013755012532515E-2</v>
+        <v>6.1878907849972013E-2</v>
       </c>
       <c r="AO10" s="18">
         <v>0</v>
       </c>
       <c r="AP10" s="18">
-        <v>0.5725190839694656</v>
+        <v>2.7752909579230081</v>
       </c>
       <c r="AQ10" s="18">
-        <v>0.29048129993180261</v>
+        <v>0.25534583610976053</v>
       </c>
       <c r="AR10" s="18">
         <v>0</v>
       </c>
       <c r="AS10" s="18">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AT10" s="18">
-        <v>0.16769230769230681</v>
+        <v>9.7152385838891693</v>
       </c>
       <c r="AU10" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AV10" s="18">
         <v>0</v>
@@ -2443,55 +2488,55 @@
         <v>86</v>
       </c>
       <c r="AX10" s="18">
-        <v>28.670256410256439</v>
+        <v>27.532067727039571</v>
       </c>
       <c r="AY10" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AZ10" s="18">
         <v>0</v>
       </c>
       <c r="BA10" s="18">
-        <v>43.664014222222207</v>
+        <v>55.051969422222221</v>
       </c>
       <c r="BB10" s="18">
-        <v>2.785636538157538E-2</v>
+        <v>0.33281321857219531</v>
       </c>
       <c r="BC10" s="18">
-        <v>6.718577777777777E-3</v>
+        <v>6.7356444444444429E-3</v>
       </c>
       <c r="BD10" s="18">
-        <v>19.684664888888889</v>
+        <v>166.87989759999999</v>
       </c>
       <c r="BE10" s="18">
-        <v>0.100551709394893</v>
+        <v>0.95338742397365739</v>
       </c>
       <c r="BF10" s="18">
         <v>0</v>
       </c>
       <c r="BG10" s="18">
-        <v>289.95555555555552</v>
+        <v>1612.6444444444439</v>
       </c>
       <c r="BH10" s="18">
-        <v>0.28501428935712891</v>
+        <v>11.012065228891339</v>
       </c>
       <c r="BI10" s="18">
-        <v>0.3</v>
+        <v>0.23333333333333331</v>
       </c>
       <c r="BJ10" s="18">
-        <v>731.78888888888878</v>
+        <v>4246.9777777777772</v>
       </c>
       <c r="BK10" s="18">
-        <v>4.8214561209185796</v>
+        <v>30.064494246623141</v>
       </c>
       <c r="BL10" s="18">
-        <v>1899614.9616640001</v>
+        <v>1894473.793536</v>
       </c>
       <c r="BM10" s="18">
-        <v>1932172.1978879999</v>
+        <v>1932173.2464640001</v>
       </c>
       <c r="BN10" s="18">
-        <v>1923397.988431819</v>
+        <v>1922446.3413184991</v>
       </c>
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.25">
@@ -2503,13 +2548,13 @@
         <v>24</v>
       </c>
       <c r="D11" s="20">
-        <v>0.13888888888889989</v>
+        <v>0.15625000000001421</v>
       </c>
       <c r="E11" s="20">
-        <v>69.340277777777786</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="F11" s="20">
-        <v>0.61983485140686412</v>
+        <v>19.6809278750166</v>
       </c>
       <c r="G11" s="20">
         <v>0</v>
@@ -2519,13 +2564,13 @@
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20">
-        <v>2.1701388888899938E-2</v>
+        <v>3.01953125</v>
       </c>
       <c r="K11" s="20">
-        <v>49.907407407407398</v>
+        <v>6.762876157407419</v>
       </c>
       <c r="L11" s="20">
-        <v>0.1215987597896913</v>
+        <v>4.0908625039434803</v>
       </c>
       <c r="M11" s="20">
         <v>0</v>
@@ -2541,40 +2586,40 @@
         <v>68.410642432000003</v>
       </c>
       <c r="R11" s="20">
-        <v>8.0902874220212198</v>
+        <v>18.446040930756212</v>
       </c>
       <c r="S11" s="20">
-        <v>23.559939616150739</v>
+        <v>24.207911031476389</v>
       </c>
       <c r="T11" s="20">
-        <v>18.70434439128427</v>
+        <v>19.80702378147372</v>
       </c>
       <c r="U11" s="20">
         <v>0</v>
       </c>
       <c r="V11" s="20">
-        <v>6.2355555555555547E-4</v>
+        <v>6.558E-4</v>
       </c>
       <c r="W11" s="20">
-        <v>4.7156233333333332E-2</v>
+        <v>13.100798122222219</v>
       </c>
       <c r="X11" s="20">
-        <v>8.9461183553811137E-4</v>
+        <v>9.3709479944849277E-3</v>
       </c>
       <c r="Y11" s="20">
-        <v>4.4366666666666663E-5</v>
+        <v>4.9933333333333332E-5</v>
       </c>
       <c r="Z11" s="20">
-        <v>2.3717831999999999</v>
+        <v>7.8494375444444433</v>
       </c>
       <c r="AA11" s="20">
-        <v>4.5722527164240127E-3</v>
+        <v>7.4333416038636357E-3</v>
       </c>
       <c r="AB11" s="20">
-        <v>1907.1004142408251</v>
+        <v>1907.203541160656</v>
       </c>
       <c r="AC11" s="20">
-        <v>2480.1078641077511</v>
+        <v>2480.2763252266909</v>
       </c>
       <c r="AD11" s="20">
         <v>0</v>
@@ -2617,67 +2662,67 @@
         <v>1</v>
       </c>
       <c r="AT11" s="20">
-        <v>6.6666666666666654E-3</v>
+        <v>52.005641025640998</v>
       </c>
       <c r="AU11" s="20">
         <v>0</v>
       </c>
       <c r="AV11" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW11" s="20">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AX11" s="20">
-        <v>29.48666666666664</v>
+        <v>28.98307692307695</v>
       </c>
       <c r="AY11" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ11" s="20">
         <v>0</v>
       </c>
       <c r="BA11" s="20">
-        <v>61.692199822222221</v>
+        <v>24.19463964444444</v>
       </c>
       <c r="BB11" s="20">
-        <v>4.4543985295358059E-2</v>
+        <v>3.2377812463398423E-2</v>
       </c>
       <c r="BC11" s="20">
-        <v>3.225599999999999E-3</v>
+        <v>1.0558577777777779E-2</v>
       </c>
       <c r="BD11" s="20">
-        <v>64.92872248888888</v>
+        <v>43.137860266666657</v>
       </c>
       <c r="BE11" s="20">
-        <v>0.20323877243107069</v>
+        <v>0.136005751646778</v>
       </c>
       <c r="BF11" s="20">
         <v>0</v>
       </c>
       <c r="BG11" s="20">
-        <v>2074.3222222222221</v>
+        <v>244.02222222222221</v>
       </c>
       <c r="BH11" s="20">
-        <v>1.373606835151147</v>
+        <v>0.55343591112374502</v>
       </c>
       <c r="BI11" s="20">
-        <v>0.31111111111111112</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="BJ11" s="20">
-        <v>1941.3888888888889</v>
+        <v>1126.9444444444439</v>
       </c>
       <c r="BK11" s="20">
-        <v>7.4001942229137061</v>
+        <v>6.1048896902648586</v>
       </c>
       <c r="BL11" s="20">
         <v>1924167.368704</v>
       </c>
       <c r="BM11" s="20">
-        <v>1930461.970432</v>
+        <v>1930453.581824</v>
       </c>
       <c r="BN11" s="20">
-        <v>1929268.7381299201</v>
+        <v>1928751.9983983589</v>
       </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.25">
@@ -2689,72 +2734,76 @@
         <v>28</v>
       </c>
       <c r="D12" s="18">
-        <v>6.9444444444457076E-2</v>
+        <v>0.104166666666686</v>
       </c>
       <c r="E12" s="18">
-        <v>30.885416666666671</v>
+        <v>83.59375</v>
       </c>
       <c r="F12" s="18">
-        <v>0.73814146639378464</v>
+        <v>79.683228237919906</v>
       </c>
       <c r="G12" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="18">
-        <v>0</v>
-      </c>
-      <c r="I12" s="18"/>
+        <v>240</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="J12" s="18">
-        <v>3.5342261904759198E-2</v>
+        <v>2.0669642857142998</v>
       </c>
       <c r="K12" s="18">
-        <v>13.71899801587303</v>
+        <v>85.896577380952294</v>
       </c>
       <c r="L12" s="18">
-        <v>0.166101130945421</v>
+        <v>30.135559799044099</v>
       </c>
       <c r="M12" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="18">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="O12" s="18">
-        <v>0</v>
-      </c>
-      <c r="P12" s="18"/>
+        <v>4</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="Q12" s="18">
         <v>137.15297484800001</v>
       </c>
       <c r="R12" s="18">
-        <v>4.4476309163256644</v>
+        <v>9.8424969104465987</v>
       </c>
       <c r="S12" s="18">
         <v>12.48751777420871</v>
       </c>
       <c r="T12" s="18">
-        <v>9.8544674040985853</v>
+        <v>10.241471263080641</v>
       </c>
       <c r="U12" s="18">
         <v>0</v>
       </c>
       <c r="V12" s="18">
-        <v>6.7012222222222217E-4</v>
+        <v>7.2015555555555544E-4</v>
       </c>
       <c r="W12" s="18">
-        <v>0.14016488888888889</v>
+        <v>1.8716937</v>
       </c>
       <c r="X12" s="18">
-        <v>9.4204722325652492E-4</v>
+        <v>2.9648822055447568E-3</v>
       </c>
       <c r="Y12" s="18">
-        <v>1.093444444444444E-4</v>
+        <v>1.100555555555555E-4</v>
       </c>
       <c r="Z12" s="18">
-        <v>3.7386433204575922</v>
+        <v>7.8984861111111098</v>
       </c>
       <c r="AA12" s="18">
-        <v>5.3859702933941444E-3</v>
+        <v>5.9691372510755391E-3</v>
       </c>
       <c r="AB12" s="18">
         <v>1063.4125556562519</v>
@@ -2800,10 +2849,10 @@
         <v>0</v>
       </c>
       <c r="AS12" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT12" s="18">
-        <v>4.6177526936890707E-3</v>
+        <v>14.0030769230769</v>
       </c>
       <c r="AU12" s="18">
         <v>0</v>
@@ -2812,10 +2861,10 @@
         <v>2</v>
       </c>
       <c r="AW12" s="18">
-        <v>57.999999999999993</v>
+        <v>36</v>
       </c>
       <c r="AX12" s="18">
-        <v>18.866598255515679</v>
+        <v>18.185128205128219</v>
       </c>
       <c r="AY12" s="18">
         <v>0</v>
@@ -2824,64 +2873,64 @@
         <v>0</v>
       </c>
       <c r="BA12" s="18">
-        <v>27.39330844444444</v>
+        <v>20.598783999999991</v>
       </c>
       <c r="BB12" s="18">
-        <v>4.0036694164287047E-2</v>
+        <v>2.7184287302262869E-2</v>
       </c>
       <c r="BC12" s="18">
-        <v>1.774933333333333E-3</v>
+        <v>2.821688888888888E-3</v>
       </c>
       <c r="BD12" s="18">
-        <v>37.829666133333333</v>
+        <v>44.114284088888887</v>
       </c>
       <c r="BE12" s="18">
-        <v>0.2102417573633984</v>
+        <v>0.1815187907830742</v>
       </c>
       <c r="BF12" s="18">
         <v>0</v>
       </c>
       <c r="BG12" s="18">
-        <v>451.15555555555551</v>
+        <v>206.83333333333329</v>
       </c>
       <c r="BH12" s="18">
-        <v>0.73371098510507626</v>
+        <v>0.65453143355250532</v>
       </c>
       <c r="BI12" s="18">
-        <v>0.2</v>
+        <v>0.25555555555555548</v>
       </c>
       <c r="BJ12" s="18">
-        <v>770.4222222222221</v>
+        <v>1529.5333333333331</v>
       </c>
       <c r="BK12" s="18">
-        <v>9.1468176592282493</v>
+        <v>9.0144836631013909</v>
       </c>
       <c r="BL12" s="18">
-        <v>872854.58534400002</v>
+        <v>880162.11148800002</v>
       </c>
       <c r="BM12" s="18">
-        <v>885193.17913599999</v>
+        <v>884953.05523199996</v>
       </c>
       <c r="BN12" s="18">
-        <v>882888.167243356</v>
+        <v>882812.11846235895</v>
       </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="20">
         <v>24</v>
       </c>
       <c r="D13" s="20">
-        <v>0.27777777777778567</v>
+        <v>12.2777777777777</v>
       </c>
       <c r="E13" s="20">
-        <v>68.159722222222229</v>
+        <v>43.656376302083302</v>
       </c>
       <c r="F13" s="20">
-        <v>4.9908118305316549</v>
+        <v>38.388587354432403</v>
       </c>
       <c r="G13" s="20">
         <v>0</v>
@@ -2891,13 +2940,13 @@
       </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20">
-        <v>1.3020833333371231E-2</v>
+        <v>4.0209780092592604</v>
       </c>
       <c r="K13" s="20">
-        <v>42.149160879629633</v>
+        <v>39.780673014322922</v>
       </c>
       <c r="L13" s="20">
-        <v>1.0093267052573369</v>
+        <v>18.821035114414201</v>
       </c>
       <c r="M13" s="20">
         <v>0</v>
@@ -2913,64 +2962,64 @@
         <v>0</v>
       </c>
       <c r="R13" s="20">
-        <v>6.1734241250517812</v>
+        <v>7.8579474317075722</v>
       </c>
       <c r="S13" s="20">
-        <v>25.053908805251549</v>
+        <v>10.41146600995569</v>
       </c>
       <c r="T13" s="20">
-        <v>11.20676467407934</v>
+        <v>7.9353826852469069</v>
       </c>
       <c r="U13" s="20">
         <v>0</v>
       </c>
       <c r="V13" s="20">
-        <v>6.6152222222222218E-4</v>
+        <v>7.0431111111111098E-4</v>
       </c>
       <c r="W13" s="20">
-        <v>0.1174056</v>
+        <v>1.4554477777777779E-2</v>
       </c>
       <c r="X13" s="20">
-        <v>5.1360275811415364E-3</v>
+        <v>1.011656942132642E-3</v>
       </c>
       <c r="Y13" s="20">
-        <v>4.6666666666666658E-5</v>
+        <v>5.0999999999999993E-5</v>
       </c>
       <c r="Z13" s="20">
-        <v>0.86345891111111106</v>
+        <v>6.150159999999999E-2</v>
       </c>
       <c r="AA13" s="20">
-        <v>6.6955637690340073E-3</v>
+        <v>1.285768816759496E-3</v>
       </c>
       <c r="AB13" s="20">
-        <v>216.76754954068349</v>
+        <v>216.13343850429229</v>
       </c>
       <c r="AC13" s="20">
-        <v>360.64158026130298</v>
+        <v>360.31434559116741</v>
       </c>
       <c r="AD13" s="20">
         <v>0</v>
       </c>
       <c r="AE13" s="20">
-        <v>0.10484775555555551</v>
+        <v>3.753968131666667E-3</v>
       </c>
       <c r="AF13" s="20">
-        <v>3.3373691975454511E-3</v>
+        <v>7.026705682098765E-5</v>
       </c>
       <c r="AG13" s="20">
-        <v>132.6490937680552</v>
+        <v>132.64664250167331</v>
       </c>
       <c r="AH13" s="20">
         <v>0</v>
       </c>
       <c r="AI13" s="20">
-        <v>8.3036888888888879E-3</v>
+        <v>5.6379243499999991E-4</v>
       </c>
       <c r="AJ13" s="20">
-        <v>3.8992745726728592E-4</v>
+        <v>1.1130156265432099E-5</v>
       </c>
       <c r="AK13" s="20">
-        <v>16.06334547626275</v>
+        <v>16.06305184547217</v>
       </c>
       <c r="AL13" s="20">
         <v>0</v>
@@ -2985,31 +3034,31 @@
         <v>0</v>
       </c>
       <c r="AP13" s="20">
-        <v>0.11115502420709419</v>
+        <v>0</v>
       </c>
       <c r="AQ13" s="20">
-        <v>6.7302299890833764E-2</v>
+        <v>0</v>
       </c>
       <c r="AR13" s="20">
         <v>0</v>
       </c>
       <c r="AS13" s="20">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AT13" s="20">
-        <v>0.8504398826979469</v>
+        <v>37.165430000000001</v>
       </c>
       <c r="AU13" s="20">
         <v>0</v>
       </c>
       <c r="AV13" s="20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW13" s="20">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="AX13" s="20">
-        <v>29.032258064516132</v>
+        <v>29.283018867924529</v>
       </c>
       <c r="AY13" s="20">
         <v>0</v>
@@ -3018,85 +3067,85 @@
         <v>0</v>
       </c>
       <c r="BA13" s="20">
-        <v>19.51769031111111</v>
+        <v>2.413556622222222</v>
       </c>
       <c r="BB13" s="20">
-        <v>0.26773522463829752</v>
+        <v>4.8563482469135791E-2</v>
       </c>
       <c r="BC13" s="20">
         <v>5.5637333333333327E-3</v>
       </c>
       <c r="BD13" s="20">
-        <v>5.7051306666666664</v>
+        <v>1.2283733333333331</v>
       </c>
       <c r="BE13" s="20">
-        <v>0.1892029662265193</v>
+        <v>4.7060565205285308E-2</v>
       </c>
       <c r="BF13" s="20">
         <v>0</v>
       </c>
       <c r="BG13" s="20">
-        <v>878.47777777777765</v>
+        <v>96.299999999999983</v>
       </c>
       <c r="BH13" s="20">
-        <v>10.506981695254421</v>
+        <v>1.939006512345679</v>
       </c>
       <c r="BI13" s="20">
-        <v>0.5888888888888888</v>
+        <v>0.6777777777777777</v>
       </c>
       <c r="BJ13" s="20">
-        <v>192.04444444444439</v>
+        <v>74.35555555555554</v>
       </c>
       <c r="BK13" s="20">
-        <v>8.9889002808319027</v>
+        <v>3.395697648219568</v>
       </c>
       <c r="BL13" s="20">
-        <v>1885356.4252160001</v>
+        <v>1886902.02624</v>
       </c>
       <c r="BM13" s="20">
-        <v>1887326.69952</v>
+        <v>1886946.0664319999</v>
       </c>
       <c r="BN13" s="20">
-        <v>1887013.0647992559</v>
+        <v>1886943.3333380739</v>
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AA14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AB14">
         <f>SUM(AB6:AB13)</f>
-        <v>10072.991540708443</v>
+        <v>10072.460556591883</v>
       </c>
       <c r="AC14">
         <f>SUM(AC6:AC13)</f>
-        <v>31608.853818835683</v>
+        <v>31608.695045284487</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AA15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AB15">
         <f>AB14/F2</f>
-        <v>4.6634220095872418E-2</v>
+        <v>4.6631761836073531E-2</v>
       </c>
       <c r="AC15">
         <f>AC14/F2</f>
-        <v>0.14633728619831335</v>
+        <v>0.14633655113557634</v>
       </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="AA16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AB16">
         <f>AB14/8/F2</f>
-        <v>5.8292775119840523E-3</v>
+        <v>5.8289702295091913E-3</v>
       </c>
       <c r="AC16">
         <f>AC14/8/F2</f>
-        <v>1.8292160774789169E-2</v>
+        <v>1.8292068891947042E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3106,19 +3155,20 @@
     <mergeCell ref="V4:AC4"/>
     <mergeCell ref="AR4:AY4"/>
     <mergeCell ref="AD4:AQ4"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:P4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BN7"/>
   <sheetViews>
@@ -3158,17 +3208,17 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3180,54 +3230,54 @@
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="38" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="26" t="s">
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="27"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="28"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -3312,20 +3362,20 @@
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="18">
         <v>8</v>
       </c>
       <c r="D6" s="18">
-        <v>5.6444444443978909</v>
+        <v>5.3999999999844874</v>
       </c>
       <c r="E6" s="18">
-        <v>28.34444444445479</v>
+        <v>12.25555555545726</v>
       </c>
       <c r="F6" s="18">
-        <v>8.2159330338296144</v>
+        <v>8.2120567995945351</v>
       </c>
       <c r="G6" s="18">
         <v>0</v>
@@ -3335,13 +3385,13 @@
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18">
-        <v>7.4583333333915363</v>
+        <v>7.5361111111285908</v>
       </c>
       <c r="K6" s="18">
-        <v>19.944444444473561</v>
+        <v>9.1611111111382826</v>
       </c>
       <c r="L6" s="18">
-        <v>7.9945090756012576</v>
+        <v>7.9990594544405269</v>
       </c>
       <c r="M6" s="18">
         <v>0</v>
@@ -3357,34 +3407,34 @@
         <v>16.525148160000001</v>
       </c>
       <c r="R6" s="18">
-        <v>58.059542045279919</v>
+        <v>58.233121656925583</v>
       </c>
       <c r="S6" s="18">
         <v>60.117016899411567</v>
       </c>
       <c r="T6" s="18">
-        <v>59.008226424226983</v>
+        <v>59.056017804054029</v>
       </c>
       <c r="U6" s="18">
         <v>0</v>
       </c>
       <c r="V6" s="18">
-        <v>3.2524055555555542E-2</v>
+        <v>3.2636966666666663E-2</v>
       </c>
       <c r="W6" s="18">
-        <v>0.26619646666666669</v>
+        <v>0.26679792222222221</v>
       </c>
       <c r="X6" s="18">
-        <v>3.7185470138552001E-2</v>
+        <v>3.7435538385227361E-2</v>
       </c>
       <c r="Y6" s="18">
-        <v>2.963742222222222E-2</v>
+        <v>2.9514211111111101E-2</v>
       </c>
       <c r="Z6" s="18">
-        <v>0.5349858666666667</v>
+        <v>0.35617500000000002</v>
       </c>
       <c r="AA6" s="18">
-        <v>3.4718308439787307E-2</v>
+        <v>3.448648880163057E-2</v>
       </c>
       <c r="AB6" s="18">
         <v>18794.08540191274</v>
@@ -3432,20 +3482,20 @@
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20">
         <v>8</v>
       </c>
       <c r="D7" s="20">
-        <v>4.2555555556383524</v>
+        <v>4.0222222222170672</v>
       </c>
       <c r="E7" s="20">
-        <v>17.877777777741571</v>
+        <v>16.288888888925111</v>
       </c>
       <c r="F7" s="20">
-        <v>8.599452937145827</v>
+        <v>8.5693464575125944</v>
       </c>
       <c r="G7" s="20">
         <v>0</v>
@@ -3455,13 +3505,13 @@
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20">
-        <v>7.1805555555490912</v>
+        <v>7.1402777777823161</v>
       </c>
       <c r="K7" s="20">
-        <v>12.32916666668544</v>
+        <v>11.12361111105808</v>
       </c>
       <c r="L7" s="20">
-        <v>8.0105795596209788</v>
+        <v>7.9450996186689622</v>
       </c>
       <c r="M7" s="20">
         <v>0</v>
@@ -3477,13 +3527,13 @@
         <v>16.818814975999999</v>
       </c>
       <c r="R7" s="20">
-        <v>36.931524277207203</v>
+        <v>37.002977967714813</v>
       </c>
       <c r="S7" s="20">
-        <v>42.865443982157522</v>
+        <v>42.694846469544757</v>
       </c>
       <c r="T7" s="20">
-        <v>39.378302261912047</v>
+        <v>39.23099558259252</v>
       </c>
       <c r="U7" s="20">
         <v>0</v>
@@ -3492,25 +3542,25 @@
         <v>3.0733777777777792E-3</v>
       </c>
       <c r="W7" s="20">
-        <v>1.581040866666666</v>
+        <v>1.3487341111111111</v>
       </c>
       <c r="X7" s="20">
-        <v>8.3461053323293566E-2</v>
+        <v>5.805612693062661E-2</v>
       </c>
       <c r="Y7" s="20">
-        <v>2.1477333333333329E-3</v>
+        <v>2.148266666666667E-3</v>
       </c>
       <c r="Z7" s="20">
-        <v>1.5729332444444439</v>
+        <v>1.341245622222222</v>
       </c>
       <c r="AA7" s="20">
-        <v>8.2381246044002432E-2</v>
+        <v>5.6750998083164493E-2</v>
       </c>
       <c r="AB7" s="20">
         <v>32008.90212566252</v>
       </c>
       <c r="AC7" s="20">
-        <v>31494.9784181305</v>
+        <v>31494.237802323249</v>
       </c>
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
@@ -3565,7 +3615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BN6"/>
   <sheetViews>
@@ -3587,17 +3637,17 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3609,9 +3659,9 @@
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3676,49 +3726,49 @@
       <c r="BN3" s="1"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>96</v>
-      </c>
       <c r="I5" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
now robust code all throuhgout e..g checking file sructure is ok
</commit_message>
<xml_diff>
--- a/data/uploaded_excel_files/uploaded_file.xlsx
+++ b/data/uploaded_excel_files/uploaded_file.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C20339A-0444-468F-AC07-2E5E5E25C7C9}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{72E707BE-0160-4B47-9423-3E839962E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83EA49F-FD48-4F55-B28D-B1775F13EF54}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="600" windowWidth="14850" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="3690" windowWidth="18900" windowHeight="9825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
-    <sheet name="VM-Data" sheetId="2" r:id="rId2"/>
-    <sheet name="MegaPort" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="WS-Data" sheetId="1" r:id="rId2"/>
+    <sheet name="VM-Data" sheetId="2" r:id="rId3"/>
+    <sheet name="MegaPort" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>Customer: 1038</t>
   </si>
@@ -360,6 +361,9 @@
     <t>ld71r16u14ws</t>
   </si>
   <si>
+    <t>4m</t>
+  </si>
+  <si>
     <t>ld71r18u44ews</t>
   </si>
   <si>
@@ -408,34 +412,13 @@
     <t>Avg</t>
   </si>
   <si>
-    <t>10m</t>
+    <t>6m</t>
+  </si>
+  <si>
+    <t>8m</t>
   </si>
   <si>
     <t>2m</t>
-  </si>
-  <si>
-    <t>ld71r18u45aws</t>
-  </si>
-  <si>
-    <t>ld71r18u44lws</t>
-  </si>
-  <si>
-    <t>6m</t>
-  </si>
-  <si>
-    <t>8m</t>
-  </si>
-  <si>
-    <t>20m</t>
-  </si>
-  <si>
-    <t>Analysis Window: Mon,Tue,Wed,Th,Fri, 20:00 to 08:00</t>
-  </si>
-  <si>
-    <t>Data Pulled: Jun 09 2024 23:00:00 - Jun 21 2024 22:59:59</t>
-  </si>
-  <si>
-    <t>ld71r18u44zws</t>
   </si>
 </sst>
 </file>
@@ -800,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,8 +837,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -873,8 +856,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -885,6 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -1211,17 +1193,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1087BDBF-61A9-4E89-AA68-4C3AF5657CC8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN19"/>
+  <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
@@ -1273,59 +1266,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
       <c r="C1" s="23"/>
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="23"/>
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22"/>
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2">
-        <v>432000</v>
+        <v>216000</v>
       </c>
     </row>
     <row r="3" spans="1:66" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="23"/>
+      <c r="A3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="22"/>
       <c r="C3" s="23"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="39" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="37" t="s">
         <v>7</v>
       </c>
       <c r="R4" s="26"/>
@@ -1387,8 +1380,8 @@
       <c r="BN4" s="26"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -1586,45 +1579,43 @@
       <c r="A6" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="18">
         <v>24</v>
       </c>
       <c r="D6" s="18">
-        <v>0.17361111111112901</v>
+        <v>3.17361111111112</v>
       </c>
       <c r="E6" s="18">
-        <v>87.7083333333333</v>
+        <v>67.708333333333343</v>
       </c>
       <c r="F6" s="18">
-        <v>76.815863962563</v>
+        <v>39.815863962563</v>
       </c>
       <c r="G6" s="18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="18">
-        <v>600</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>99</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I6" s="18"/>
       <c r="J6" s="18">
-        <v>1.3176204919673751E-2</v>
+        <v>2.0131762049196702</v>
       </c>
       <c r="K6" s="18">
-        <v>86.9639756944444</v>
+        <v>28.9639756944444</v>
       </c>
       <c r="L6" s="18">
-        <v>77.080784774711404</v>
+        <v>18.0807847747114</v>
       </c>
       <c r="M6" s="18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N6" s="18">
-        <v>600</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>99</v>
+        <v>0</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0</v>
       </c>
       <c r="P6" s="18"/>
       <c r="Q6" s="18">
@@ -1701,13 +1692,13 @@
         <v>0</v>
       </c>
       <c r="AR6" s="18">
-        <v>2.0390000000000001</v>
+        <v>0</v>
       </c>
       <c r="AS6" s="18">
-        <v>85.674000000000007</v>
+        <v>0</v>
       </c>
       <c r="AT6" s="18">
-        <v>72.6721</v>
+        <v>20.1234</v>
       </c>
       <c r="AU6" s="18">
         <v>0</v>
@@ -1774,45 +1765,49 @@
       <c r="A7" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="20">
         <v>28</v>
       </c>
       <c r="D7" s="20">
-        <v>2.55555555555557</v>
+        <v>1.55555555555557</v>
       </c>
       <c r="E7" s="20">
-        <v>38.2638888888889</v>
+        <v>88.2638888888889</v>
       </c>
       <c r="F7" s="20">
-        <v>13.7140567507901</v>
+        <v>24.7140567507901</v>
       </c>
       <c r="G7" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="20">
-        <v>0</v>
-      </c>
-      <c r="I7" s="20"/>
+        <v>120</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="J7" s="20">
-        <v>6.2624007936506132E-2</v>
+        <v>9.0626240079365008</v>
       </c>
       <c r="K7" s="20">
-        <v>36.690228174603099</v>
+        <v>89.690228174603106</v>
       </c>
       <c r="L7" s="20">
-        <v>10.132013670350799</v>
+        <v>89.132013670350801</v>
       </c>
       <c r="M7" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="20">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="O7" s="20">
-        <v>0</v>
-      </c>
-      <c r="P7" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="Q7" s="20">
         <v>137.15297484800001</v>
       </c>
@@ -1887,13 +1882,13 @@
         <v>0</v>
       </c>
       <c r="AR7" s="20">
-        <v>4.8467000000000002</v>
+        <v>0</v>
       </c>
       <c r="AS7" s="20">
-        <v>37.213000000000001</v>
+        <v>3</v>
       </c>
       <c r="AT7" s="20">
-        <v>20.005128205128202</v>
+        <v>13.54321</v>
       </c>
       <c r="AU7" s="20">
         <v>0</v>
@@ -1960,45 +1955,43 @@
       <c r="A8" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="18">
         <v>24</v>
       </c>
       <c r="D8" s="18">
-        <v>0.32986111111111432</v>
+        <v>2.3298611111111098</v>
       </c>
       <c r="E8" s="18">
-        <v>86.4756944444444</v>
+        <v>76.475694444444443</v>
       </c>
       <c r="F8" s="18">
-        <v>75.922552346485602</v>
+        <v>13.922552346485629</v>
       </c>
       <c r="G8" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="18">
-        <v>360</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>103</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I8" s="18"/>
       <c r="J8" s="18">
-        <v>2.0376157407407001</v>
+        <v>3.7615740740747597E-2</v>
       </c>
       <c r="K8" s="18">
-        <v>85.690732666015606</v>
+        <v>25.69073266601562</v>
       </c>
       <c r="L8" s="18">
-        <v>72.374675111090795</v>
+        <v>15.3746751110908</v>
       </c>
       <c r="M8" s="18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N8" s="18">
-        <v>360</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>103</v>
+        <v>0</v>
+      </c>
+      <c r="O8" s="18">
+        <v>0</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="18">
@@ -2083,13 +2076,13 @@
         <v>8.85484379787249E-2</v>
       </c>
       <c r="AR8" s="18">
-        <v>3.7320000000000002</v>
+        <v>0</v>
       </c>
       <c r="AS8" s="18">
-        <v>86.975999999999999</v>
+        <v>46</v>
       </c>
       <c r="AT8" s="18">
-        <v>74.121087737301295</v>
+        <v>4.1210877373013304</v>
       </c>
       <c r="AU8" s="18">
         <v>0</v>
@@ -2152,22 +2145,22 @@
         <v>1903922.5645696661</v>
       </c>
     </row>
-    <row r="9" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="21"/>
+        <v>79</v>
+      </c>
+      <c r="B9" s="19"/>
       <c r="C9" s="20">
         <v>28</v>
       </c>
       <c r="D9" s="20">
-        <v>3.2604166666666701</v>
+        <v>0.2604166666666714</v>
       </c>
       <c r="E9" s="20">
-        <v>63.8715277777778</v>
+        <v>63.871527777777779</v>
       </c>
       <c r="F9" s="20">
-        <v>52.460464852049299</v>
+        <v>0.460464852049355</v>
       </c>
       <c r="G9" s="20">
         <v>0</v>
@@ -2177,24 +2170,26 @@
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20">
-        <v>5.0365823412698596</v>
+        <v>2.03658234126986</v>
       </c>
       <c r="K9" s="20">
-        <v>67.5086805555555</v>
+        <v>97.5086805555555</v>
       </c>
       <c r="L9" s="20">
-        <v>53.128619426852701</v>
+        <v>79.128619426852694</v>
       </c>
       <c r="M9" s="20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N9" s="20">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="O9" s="20">
-        <v>0</v>
-      </c>
-      <c r="P9" s="20"/>
+        <v>5</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>101</v>
+      </c>
       <c r="Q9" s="20">
         <v>137.15297484800001</v>
       </c>
@@ -2277,13 +2272,13 @@
         <v>0</v>
       </c>
       <c r="AR9" s="20">
-        <v>4.6289999999999996</v>
+        <v>0</v>
       </c>
       <c r="AS9" s="20">
-        <v>69.018000000000001</v>
+        <v>9</v>
       </c>
       <c r="AT9" s="20">
-        <v>50.004615384615299</v>
+        <v>71.004615384615306</v>
       </c>
       <c r="AU9" s="20">
         <v>0</v>
@@ -2346,51 +2341,53 @@
         <v>874526.4324986093</v>
       </c>
     </row>
-    <row r="10" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="21"/>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="18">
         <v>24</v>
       </c>
       <c r="D10" s="18">
-        <v>9.1215277777777803</v>
+        <v>16.1215277777777</v>
       </c>
       <c r="E10" s="18">
-        <v>92.208333333333002</v>
+        <v>98.2083333333333</v>
       </c>
       <c r="F10" s="18">
-        <v>89.7926838412546</v>
+        <v>72.7926838412546</v>
       </c>
       <c r="G10" s="18">
+        <v>3</v>
+      </c>
+      <c r="H10" s="18">
+        <v>360</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="18">
+        <v>13.0224247685185</v>
+      </c>
+      <c r="K10" s="18">
+        <v>99.7157118055556</v>
+      </c>
+      <c r="L10" s="18">
+        <v>76.9876</v>
+      </c>
+      <c r="M10" s="18">
         <v>4</v>
       </c>
-      <c r="H10" s="18">
+      <c r="N10" s="18">
         <v>480</v>
       </c>
-      <c r="I10" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="18">
-        <v>3.0224247685185301</v>
-      </c>
-      <c r="K10" s="18">
-        <v>96.7157118055556</v>
-      </c>
-      <c r="L10" s="18">
-        <v>88.445829334338995</v>
-      </c>
-      <c r="M10" s="18">
-        <v>0</v>
-      </c>
-      <c r="N10" s="18">
-        <v>0</v>
-      </c>
       <c r="O10" s="18">
-        <v>0</v>
-      </c>
-      <c r="P10" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>101</v>
+      </c>
       <c r="Q10" s="18">
         <v>68.410642432000003</v>
       </c>
@@ -2473,13 +2470,13 @@
         <v>0.25534583610976053</v>
       </c>
       <c r="AR10" s="18">
-        <v>0.192</v>
+        <v>0</v>
       </c>
       <c r="AS10" s="18">
-        <v>95.234566999999998</v>
+        <v>95</v>
       </c>
       <c r="AT10" s="18">
-        <v>87.715238583889104</v>
+        <v>9.7152385838891693</v>
       </c>
       <c r="AU10" s="18">
         <v>3</v>
@@ -2542,49 +2539,47 @@
         <v>1922446.3413184991</v>
       </c>
     </row>
-    <row r="11" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="21"/>
+        <v>81</v>
+      </c>
+      <c r="B11" s="19"/>
       <c r="C11" s="20">
         <v>24</v>
       </c>
       <c r="D11" s="20">
-        <v>19.15625</v>
+        <v>0.15625000000001421</v>
       </c>
       <c r="E11" s="20">
-        <v>99.6666666666667</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="F11" s="20">
-        <v>80.680927875016593</v>
+        <v>19.6809278750166</v>
       </c>
       <c r="G11" s="20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11" s="20">
-        <v>1200</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>105</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I11" s="20"/>
       <c r="J11" s="20">
-        <v>20.01953125</v>
+        <v>3.01953125</v>
       </c>
       <c r="K11" s="20">
-        <v>96.762876157407405</v>
+        <v>6.762876157407419</v>
       </c>
       <c r="L11" s="20">
-        <v>83.090862503943399</v>
+        <v>4.0908625039434803</v>
       </c>
       <c r="M11" s="20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N11" s="20">
-        <v>1200</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="O11" s="20">
+        <v>0</v>
       </c>
       <c r="P11" s="20"/>
       <c r="Q11" s="20">
@@ -2661,13 +2656,13 @@
         <v>0</v>
       </c>
       <c r="AR11" s="20">
-        <v>1.9279999999999999</v>
+        <v>0</v>
       </c>
       <c r="AS11" s="20">
-        <v>96.417000000000002</v>
+        <v>1</v>
       </c>
       <c r="AT11" s="20">
-        <v>82.005641025640998</v>
+        <v>52.005641025640998</v>
       </c>
       <c r="AU11" s="20">
         <v>0</v>
@@ -2731,50 +2726,52 @@
       </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="21"/>
+      <c r="A12" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="17"/>
       <c r="C12" s="18">
         <v>28</v>
       </c>
       <c r="D12" s="18">
-        <v>18.1041666666666</v>
+        <v>0.104166666666686</v>
       </c>
       <c r="E12" s="18">
-        <v>97.59375</v>
+        <v>83.59375</v>
       </c>
       <c r="F12" s="18">
-        <v>50.683228237919899</v>
+        <v>79.683228237919906</v>
       </c>
       <c r="G12" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="18">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="J12" s="18">
-        <v>6.6964285714306016E-2</v>
+        <v>2.0669642857142998</v>
       </c>
       <c r="K12" s="18">
-        <v>95.896577380952294</v>
+        <v>85.896577380952294</v>
       </c>
       <c r="L12" s="18">
-        <v>49.135559799044103</v>
+        <v>30.135559799044099</v>
       </c>
       <c r="M12" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="18">
-        <v>120</v>
-      </c>
-      <c r="O12" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="P12" s="18"/>
+        <v>240</v>
+      </c>
+      <c r="O12" s="18">
+        <v>4</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="Q12" s="18">
         <v>137.15297484800001</v>
       </c>
@@ -2849,13 +2846,13 @@
         <v>0</v>
       </c>
       <c r="AR12" s="18">
-        <v>7.8289999999999997</v>
+        <v>0</v>
       </c>
       <c r="AS12" s="18">
-        <v>94.781899999999993</v>
+        <v>1</v>
       </c>
       <c r="AT12" s="18">
-        <v>45.003076923076897</v>
+        <v>14.0030769230769</v>
       </c>
       <c r="AU12" s="18">
         <v>0</v>
@@ -2919,21 +2916,21 @@
       </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="21"/>
+      <c r="A13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="19"/>
       <c r="C13" s="20">
         <v>24</v>
       </c>
       <c r="D13" s="20">
-        <v>0.27777777777778567</v>
+        <v>12.2777777777777</v>
       </c>
       <c r="E13" s="20">
-        <v>40.656376302083331</v>
+        <v>43.656376302083302</v>
       </c>
       <c r="F13" s="20">
-        <v>1.3885873544324741</v>
+        <v>38.388587354432403</v>
       </c>
       <c r="G13" s="20">
         <v>0</v>
@@ -2943,13 +2940,13 @@
       </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20">
-        <v>2.0978009259266631E-2</v>
+        <v>4.0209780092592604</v>
       </c>
       <c r="K13" s="20">
-        <v>39.7806730143229</v>
+        <v>39.780673014322922</v>
       </c>
       <c r="L13" s="20">
-        <v>4.82103511441424</v>
+        <v>18.821035114414201</v>
       </c>
       <c r="M13" s="20">
         <v>0</v>
@@ -3043,13 +3040,13 @@
         <v>0</v>
       </c>
       <c r="AR13" s="20">
-        <v>0.81899999999999995</v>
+        <v>0</v>
       </c>
       <c r="AS13" s="20">
-        <v>34.173000000000002</v>
+        <v>0</v>
       </c>
       <c r="AT13" s="20">
-        <v>1.9283699999999999</v>
+        <v>37.165430000000001</v>
       </c>
       <c r="AU13" s="20">
         <v>0</v>
@@ -3113,624 +3110,42 @@
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="20">
-        <v>24</v>
-      </c>
-      <c r="D14" s="20">
-        <v>0.27777777777778567</v>
-      </c>
-      <c r="E14" s="20">
-        <v>50.656376302083302</v>
-      </c>
-      <c r="F14" s="20">
-        <v>2.3885873544324698</v>
-      </c>
-      <c r="G14" s="20">
-        <v>0</v>
-      </c>
-      <c r="H14" s="20">
-        <v>0</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20">
-        <v>2.0978009259266631E-2</v>
-      </c>
-      <c r="K14" s="20">
-        <v>59.7806730143229</v>
-      </c>
-      <c r="L14" s="20">
-        <v>3.82103511441424</v>
-      </c>
-      <c r="M14" s="20">
-        <v>0</v>
-      </c>
-      <c r="N14" s="20">
-        <v>0</v>
-      </c>
-      <c r="O14" s="20">
-        <v>0</v>
-      </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20">
-        <v>0</v>
-      </c>
-      <c r="R14" s="20">
-        <v>7.8579474317075722</v>
-      </c>
-      <c r="S14" s="20">
-        <v>10.41146600995569</v>
-      </c>
-      <c r="T14" s="20">
-        <v>7.9353826852469069</v>
-      </c>
-      <c r="U14" s="20">
-        <v>0</v>
-      </c>
-      <c r="V14" s="20">
-        <v>7.0431111111111098E-4</v>
-      </c>
-      <c r="W14" s="20">
-        <v>1.4554477777777779E-2</v>
-      </c>
-      <c r="X14" s="20">
-        <v>1.011656942132642E-3</v>
-      </c>
-      <c r="Y14" s="20">
-        <v>5.0999999999999993E-5</v>
-      </c>
-      <c r="Z14" s="20">
-        <v>6.150159999999999E-2</v>
-      </c>
-      <c r="AA14" s="20">
-        <v>1.285768816759496E-3</v>
-      </c>
-      <c r="AB14" s="20">
-        <v>216.13343850429229</v>
-      </c>
-      <c r="AC14" s="20">
-        <v>360.31434559116741</v>
-      </c>
-      <c r="AD14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="20">
-        <v>3.753968131666667E-3</v>
-      </c>
-      <c r="AF14" s="20">
-        <v>7.026705682098765E-5</v>
-      </c>
-      <c r="AG14" s="20">
-        <v>132.64664250167331</v>
-      </c>
-      <c r="AH14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="20">
-        <v>5.6379243499999991E-4</v>
-      </c>
-      <c r="AJ14" s="20">
-        <v>1.1130156265432099E-5</v>
-      </c>
-      <c r="AK14" s="20">
-        <v>16.06305184547217</v>
-      </c>
-      <c r="AL14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="20">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="AS14" s="20">
-        <v>44.173000000000002</v>
-      </c>
-      <c r="AT14" s="20">
-        <v>19.928370000000001</v>
-      </c>
-      <c r="AU14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AV14" s="20">
-        <v>9</v>
-      </c>
-      <c r="AW14" s="20">
-        <v>45</v>
-      </c>
-      <c r="AX14" s="20">
-        <v>29.283018867924529</v>
-      </c>
-      <c r="AY14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="20">
-        <v>0</v>
-      </c>
-      <c r="BA14" s="20">
-        <v>2.413556622222222</v>
-      </c>
-      <c r="BB14" s="20">
-        <v>4.8563482469135791E-2</v>
-      </c>
-      <c r="BC14" s="20">
-        <v>5.5637333333333327E-3</v>
-      </c>
-      <c r="BD14" s="20">
-        <v>1.2283733333333331</v>
-      </c>
-      <c r="BE14" s="20">
-        <v>4.7060565205285308E-2</v>
-      </c>
-      <c r="BF14" s="20">
-        <v>0</v>
-      </c>
-      <c r="BG14" s="20">
-        <v>96.299999999999983</v>
-      </c>
-      <c r="BH14" s="20">
-        <v>1.939006512345679</v>
-      </c>
-      <c r="BI14" s="20">
-        <v>0.6777777777777777</v>
-      </c>
-      <c r="BJ14" s="20">
-        <v>74.35555555555554</v>
-      </c>
-      <c r="BK14" s="20">
-        <v>3.395697648219568</v>
-      </c>
-      <c r="BL14" s="20">
-        <v>1886902.02624</v>
-      </c>
-      <c r="BM14" s="20">
-        <v>1886946.0664319999</v>
-      </c>
-      <c r="BN14" s="20">
-        <v>1886943.3333380739</v>
+      <c r="AA14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB14">
+        <f>SUM(AB6:AB13)</f>
+        <v>10072.460556591883</v>
+      </c>
+      <c r="AC14">
+        <f>SUM(AC6:AC13)</f>
+        <v>31608.695045284487</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="20">
-        <v>24</v>
-      </c>
-      <c r="D15" s="20">
-        <v>0.27777777777778567</v>
-      </c>
-      <c r="E15" s="20">
-        <v>30.656376302083299</v>
-      </c>
-      <c r="F15" s="20">
-        <v>3.3885873544324698</v>
-      </c>
-      <c r="G15" s="20">
-        <v>0</v>
-      </c>
-      <c r="H15" s="20">
-        <v>0</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20">
-        <v>2.0978009259266631E-2</v>
-      </c>
-      <c r="K15" s="20">
-        <v>29.7806730143229</v>
-      </c>
-      <c r="L15" s="20">
-        <v>1.82103511441424</v>
-      </c>
-      <c r="M15" s="20">
-        <v>0</v>
-      </c>
-      <c r="N15" s="20">
-        <v>0</v>
-      </c>
-      <c r="O15" s="20">
-        <v>0</v>
-      </c>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20">
-        <v>0</v>
-      </c>
-      <c r="R15" s="20">
-        <v>7.8579474317075722</v>
-      </c>
-      <c r="S15" s="20">
-        <v>10.41146600995569</v>
-      </c>
-      <c r="T15" s="20">
-        <v>7.9353826852469069</v>
-      </c>
-      <c r="U15" s="20">
-        <v>0</v>
-      </c>
-      <c r="V15" s="20">
-        <v>7.0431111111111098E-4</v>
-      </c>
-      <c r="W15" s="20">
-        <v>1.4554477777777779E-2</v>
-      </c>
-      <c r="X15" s="20">
-        <v>1.011656942132642E-3</v>
-      </c>
-      <c r="Y15" s="20">
-        <v>5.0999999999999993E-5</v>
-      </c>
-      <c r="Z15" s="20">
-        <v>6.150159999999999E-2</v>
-      </c>
-      <c r="AA15" s="20">
-        <v>1.285768816759496E-3</v>
-      </c>
-      <c r="AB15" s="20">
-        <v>216.13343850429229</v>
-      </c>
-      <c r="AC15" s="20">
-        <v>360.31434559116741</v>
-      </c>
-      <c r="AD15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="20">
-        <v>3.753968131666667E-3</v>
-      </c>
-      <c r="AF15" s="20">
-        <v>7.026705682098765E-5</v>
-      </c>
-      <c r="AG15" s="20">
-        <v>132.64664250167331</v>
-      </c>
-      <c r="AH15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="20">
-        <v>5.6379243499999991E-4</v>
-      </c>
-      <c r="AJ15" s="20">
-        <v>1.1130156265432099E-5</v>
-      </c>
-      <c r="AK15" s="20">
-        <v>16.06305184547217</v>
-      </c>
-      <c r="AL15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AN15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AO15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="20">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="AS15" s="20">
-        <v>24.172999999999998</v>
-      </c>
-      <c r="AT15" s="20">
-        <v>5.9283700000000001</v>
-      </c>
-      <c r="AU15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AV15" s="20">
-        <v>9</v>
-      </c>
-      <c r="AW15" s="20">
-        <v>45</v>
-      </c>
-      <c r="AX15" s="20">
-        <v>29.283018867924529</v>
-      </c>
-      <c r="AY15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="20">
-        <v>0</v>
-      </c>
-      <c r="BA15" s="20">
-        <v>2.413556622222222</v>
-      </c>
-      <c r="BB15" s="20">
-        <v>4.8563482469135791E-2</v>
-      </c>
-      <c r="BC15" s="20">
-        <v>5.5637333333333327E-3</v>
-      </c>
-      <c r="BD15" s="20">
-        <v>1.2283733333333331</v>
-      </c>
-      <c r="BE15" s="20">
-        <v>4.7060565205285308E-2</v>
-      </c>
-      <c r="BF15" s="20">
-        <v>0</v>
-      </c>
-      <c r="BG15" s="20">
-        <v>96.299999999999983</v>
-      </c>
-      <c r="BH15" s="20">
-        <v>1.939006512345679</v>
-      </c>
-      <c r="BI15" s="20">
-        <v>0.6777777777777777</v>
-      </c>
-      <c r="BJ15" s="20">
-        <v>74.35555555555554</v>
-      </c>
-      <c r="BK15" s="20">
-        <v>3.395697648219568</v>
-      </c>
-      <c r="BL15" s="20">
-        <v>1886902.02624</v>
-      </c>
-      <c r="BM15" s="20">
-        <v>1886946.0664319999</v>
-      </c>
-      <c r="BN15" s="20">
-        <v>1886943.3333380739</v>
+      <c r="AA15" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB15">
+        <f>AB14/F2</f>
+        <v>4.6631761836073531E-2</v>
+      </c>
+      <c r="AC15">
+        <f>AC14/F2</f>
+        <v>0.14633655113557634</v>
       </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="20">
-        <v>24</v>
-      </c>
-      <c r="D16" s="20">
-        <v>2.8193000000000001</v>
-      </c>
-      <c r="E16" s="20">
-        <v>75.656376302083302</v>
-      </c>
-      <c r="F16" s="20">
-        <v>61.388587354432403</v>
-      </c>
-      <c r="G16" s="20">
-        <v>0</v>
-      </c>
-      <c r="H16" s="20">
-        <v>0</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20">
-        <v>8.0209780092592595</v>
-      </c>
-      <c r="K16" s="20">
-        <v>79.7806730143229</v>
-      </c>
-      <c r="L16" s="20">
-        <v>69.821035114414201</v>
-      </c>
-      <c r="M16" s="20">
-        <v>0</v>
-      </c>
-      <c r="N16" s="20">
-        <v>0</v>
-      </c>
-      <c r="O16" s="20">
-        <v>0</v>
-      </c>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20">
-        <v>0</v>
-      </c>
-      <c r="R16" s="20">
-        <v>7.8579474317075722</v>
-      </c>
-      <c r="S16" s="20">
-        <v>10.41146600995569</v>
-      </c>
-      <c r="T16" s="20">
-        <v>7.9353826852469069</v>
-      </c>
-      <c r="U16" s="20">
-        <v>0</v>
-      </c>
-      <c r="V16" s="20">
-        <v>7.0431111111111098E-4</v>
-      </c>
-      <c r="W16" s="20">
-        <v>1.4554477777777779E-2</v>
-      </c>
-      <c r="X16" s="20">
-        <v>1.011656942132642E-3</v>
-      </c>
-      <c r="Y16" s="20">
-        <v>5.0999999999999993E-5</v>
-      </c>
-      <c r="Z16" s="20">
-        <v>6.150159999999999E-2</v>
-      </c>
-      <c r="AA16" s="20">
-        <v>1.285768816759496E-3</v>
-      </c>
-      <c r="AB16" s="20">
-        <v>216.13343850429229</v>
-      </c>
-      <c r="AC16" s="20">
-        <v>360.31434559116741</v>
-      </c>
-      <c r="AD16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="20">
-        <v>3.753968131666667E-3</v>
-      </c>
-      <c r="AF16" s="20">
-        <v>7.026705682098765E-5</v>
-      </c>
-      <c r="AG16" s="20">
-        <v>132.64664250167331</v>
-      </c>
-      <c r="AH16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="20">
-        <v>5.6379243499999991E-4</v>
-      </c>
-      <c r="AJ16" s="20">
-        <v>1.1130156265432099E-5</v>
-      </c>
-      <c r="AK16" s="20">
-        <v>16.06305184547217</v>
-      </c>
-      <c r="AL16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AN16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AO16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AR16" s="20">
-        <v>20.137799999999999</v>
-      </c>
-      <c r="AS16" s="20">
-        <v>75.764300000000006</v>
-      </c>
-      <c r="AT16" s="20">
-        <v>59.987653999999999</v>
-      </c>
-      <c r="AU16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AV16" s="20">
-        <v>9</v>
-      </c>
-      <c r="AW16" s="20">
-        <v>45</v>
-      </c>
-      <c r="AX16" s="20">
-        <v>29.283018867924529</v>
-      </c>
-      <c r="AY16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AZ16" s="20">
-        <v>0</v>
-      </c>
-      <c r="BA16" s="20">
-        <v>2.413556622222222</v>
-      </c>
-      <c r="BB16" s="20">
-        <v>4.8563482469135791E-2</v>
-      </c>
-      <c r="BC16" s="20">
-        <v>5.5637333333333327E-3</v>
-      </c>
-      <c r="BD16" s="20">
-        <v>1.2283733333333331</v>
-      </c>
-      <c r="BE16" s="20">
-        <v>4.7060565205285308E-2</v>
-      </c>
-      <c r="BF16" s="20">
-        <v>0</v>
-      </c>
-      <c r="BG16" s="20">
-        <v>96.299999999999983</v>
-      </c>
-      <c r="BH16" s="20">
-        <v>1.939006512345679</v>
-      </c>
-      <c r="BI16" s="20">
-        <v>0.6777777777777777</v>
-      </c>
-      <c r="BJ16" s="20">
-        <v>74.35555555555554</v>
-      </c>
-      <c r="BK16" s="20">
-        <v>3.395697648219568</v>
-      </c>
-      <c r="BL16" s="20">
-        <v>1886902.02624</v>
-      </c>
-      <c r="BM16" s="20">
-        <v>1886946.0664319999</v>
-      </c>
-      <c r="BN16" s="20">
-        <v>1886943.3333380739</v>
-      </c>
-    </row>
-    <row r="17" spans="27:29" x14ac:dyDescent="0.25">
-      <c r="AA17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB17">
-        <f>SUM(AB6:AB16)</f>
-        <v>10720.860872104759</v>
-      </c>
-      <c r="AC17">
-        <f>SUM(AC6:AC16)</f>
-        <v>32689.638082057987</v>
-      </c>
-    </row>
-    <row r="18" spans="27:29" x14ac:dyDescent="0.25">
-      <c r="AA18" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB18">
-        <f>AB17/F2</f>
-        <v>2.481680757431657E-2</v>
-      </c>
-      <c r="AC18">
-        <f>AC17/F2</f>
-        <v>7.5670458523282372E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="27:29" x14ac:dyDescent="0.25">
-      <c r="AA19" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB19">
-        <f>AB17/8/F2</f>
-        <v>3.1021009467895712E-3</v>
-      </c>
-      <c r="AC19">
-        <f>AC17/8/F2</f>
-        <v>9.4588073154102965E-3</v>
+      <c r="AA16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB16">
+        <f>AB14/8/F2</f>
+        <v>5.8289702295091913E-3</v>
+      </c>
+      <c r="AC16">
+        <f>AC14/8/F2</f>
+        <v>1.8292068891947042E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3740,12 +3155,12 @@
     <mergeCell ref="V4:AC4"/>
     <mergeCell ref="AR4:AY4"/>
     <mergeCell ref="AD4:AQ4"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:P4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3753,7 +3168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BN7"/>
   <sheetViews>
@@ -3790,7 +3205,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="23"/>
@@ -3798,7 +3213,7 @@
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="23"/>
@@ -3812,7 +3227,7 @@
       </c>
     </row>
     <row r="3" spans="1:66" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="23"/>
@@ -3820,29 +3235,29 @@
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="39" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="37" t="s">
         <v>7</v>
       </c>
       <c r="R4" s="26"/>
@@ -3861,8 +3276,8 @@
       <c r="AC4" s="28"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -3947,7 +3362,7 @@
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="18">
@@ -4067,7 +3482,7 @@
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20">
@@ -4200,7 +3615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BN6"/>
   <sheetViews>
@@ -4219,7 +3634,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="23"/>
@@ -4227,7 +3642,7 @@
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="23"/>
@@ -4241,7 +3656,7 @@
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="23"/>
@@ -4311,49 +3726,49 @@
       <c r="BN3" s="1"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="43" t="s">
+      <c r="A4" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="44" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="42" t="s">
         <v>92</v>
+      </c>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>96</v>
-      </c>
       <c r="I5" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">

</xml_diff>